<commit_message>
Se modifio el tab 4
</commit_message>
<xml_diff>
--- a/output/resultadosCompuTrabajo.xlsx
+++ b/output/resultadosCompuTrabajo.xlsx
@@ -442,7 +442,7 @@
         <v>A convenir</v>
       </c>
       <c r="F2" t="str">
-        <v>Hace 57 minutos (actualizada)</v>
+        <v>Hace 1 hora (actualizada)</v>
       </c>
       <c r="G2" t="str" xml:space="preserve">
         <v xml:space="preserve">Buscamos un barrendero para tareas de limpieza y mantenimiento de áreas comunes.
@@ -512,7 +512,7 @@
         <v>$ 10,000.00 (Mensual)</v>
       </c>
       <c r="F4" t="str">
-        <v>Hace 21 horas (actualizada)</v>
+        <v>Hace 22 horas (actualizada)</v>
       </c>
       <c r="G4" t="str" xml:space="preserve">
         <v xml:space="preserve">Importante empresa de MANTENIMIENTO está en busca de tu talento
@@ -547,7 +547,7 @@
         <v>$ 8,000.00 (Mensual)</v>
       </c>
       <c r="F5" t="str">
-        <v>Hace 21 horas (actualizada)</v>
+        <v>Hace 22 horas (actualizada)</v>
       </c>
       <c r="G5" t="str" xml:space="preserve">
         <v xml:space="preserve">Importante empresa de MANTENIMIENTO está en busca de tu talento

</xml_diff>

<commit_message>
[ADD]: se añadieron los cambios chidos de los mapas
</commit_message>
<xml_diff>
--- a/output/resultadosCompuTrabajo.xlsx
+++ b/output/resultadosCompuTrabajo.xlsx
@@ -442,7 +442,7 @@
         <v>A convenir</v>
       </c>
       <c r="F2" t="str">
-        <v>Hace 1 hora (actualizada)</v>
+        <v>Hace 2 horas (actualizada)</v>
       </c>
       <c r="G2" t="str" xml:space="preserve">
         <v xml:space="preserve">Buscamos un barrendero para tareas de limpieza y mantenimiento de áreas comunes.
@@ -474,7 +474,7 @@
         <v>$ 10,000.00 (Mensual)</v>
       </c>
       <c r="F3" t="str">
-        <v>Hace 9 horas (actualizada)</v>
+        <v>Hace 10 horas (actualizada)</v>
       </c>
       <c r="G3" t="str" xml:space="preserve">
         <v xml:space="preserve">Importante mercado está en busca de tu talento

</xml_diff>